<commit_message>
adding photometric data, single measurement point of natural far red outdoors upon sunrise
</commit_message>
<xml_diff>
--- a/prj/hazelnut_large/LHC-001/6-Photometric Test Data/2019-03-21_tests.xlsx
+++ b/prj/hazelnut_large/LHC-001/6-Photometric Test Data/2019-03-21_tests.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsavas/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsavas/Documents/git/openag-mechanical/prj/hazelnut_large/LHC-001/6-Photometric Test Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2B45EF-9994-7248-82EE-FEE74AC82781}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5BEE7B-7EEA-C246-8A98-40E049B2C745}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test01" sheetId="2" r:id="rId1"/>
     <sheet name="test02" sheetId="3" r:id="rId2"/>
     <sheet name="12&quot;_4x COB_scratch" sheetId="11" state="hidden" r:id="rId3"/>
-    <sheet name="metadata" sheetId="12" r:id="rId4"/>
+    <sheet name="test03" sheetId="13" r:id="rId4"/>
+    <sheet name="metadata" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Target Wall, Warehouse</t>
   </si>
@@ -101,6 +102,30 @@
   </si>
   <si>
     <t>Tab describes 6 COB including far red, with 1825 optic, at 18" from target wall; first plot shows full PAR range, second plot shows far red range</t>
+  </si>
+  <si>
+    <t>Sunrise Measurement</t>
+  </si>
+  <si>
+    <t>2019-03-29 8:12 a.m.</t>
+  </si>
+  <si>
+    <t>Location: MIT Bates warehouse lot</t>
+  </si>
+  <si>
+    <t>Far red (701-780nm): 6.83 µmol/m2/s</t>
+  </si>
+  <si>
+    <t>PPFD (400-700nm): 174.72 µmol/m2/s</t>
+  </si>
+  <si>
+    <t>test03</t>
+  </si>
+  <si>
+    <t>Tab describes a single data point taken outdoors during sunrise, for far red comparison.</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -111,7 +136,7 @@
     <numFmt numFmtId="164" formatCode="###0"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -153,6 +178,20 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -168,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -256,11 +295,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -402,6 +521,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +875,7 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N3" sqref="N1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -730,6 +884,7 @@
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="12" width="7.33203125" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
     <col min="15" max="16384" width="14.5" hidden="1"/>
   </cols>
   <sheetData>
@@ -1149,7 +1304,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD1048576"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
@@ -1157,6 +1312,7 @@
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="12" width="7.33203125" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
     <col min="15" max="16384" width="14.5" hidden="1"/>
   </cols>
   <sheetData>
@@ -2727,14 +2883,175 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68676DBE-26A5-EF41-8BFB-47536DAF406E}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="14.5" style="52" customWidth="1"/>
+    <col min="2" max="10" width="7.33203125" style="52" customWidth="1"/>
+    <col min="11" max="11" width="0" style="52" hidden="1" customWidth="1"/>
+    <col min="12" max="14" width="0" style="52" hidden="1"/>
+    <col min="15" max="16384" width="14.5" style="52" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="51"/>
+      <c r="K1" s="53"/>
+    </row>
+    <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="51"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="51"/>
+      <c r="B3" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="55"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="53"/>
+    </row>
+    <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="51"/>
+      <c r="B4" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="51"/>
+      <c r="B5" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="51"/>
+      <c r="K6" s="53"/>
+    </row>
+    <row r="7" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="51"/>
+      <c r="B7" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="61"/>
+      <c r="K7" s="53"/>
+    </row>
+    <row r="8" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="51"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="64"/>
+      <c r="K8" s="53"/>
+    </row>
+    <row r="9" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="51"/>
+      <c r="B9" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="51"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <conditionalFormatting sqref="H9:J9 B11:J11">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FFCC0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:J9 B11:J11">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FF57BB8A"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
@@ -2808,9 +3125,15 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="48"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="46"/>
+      <c r="A8" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="48"/>

</xml_diff>